<commit_message>
fixing dowload file corupt
</commit_message>
<xml_diff>
--- a/files/Kepaniteraan Hukum.xlsx
+++ b/files/Kepaniteraan Hukum.xlsx
@@ -368,412 +368,207 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>a</v>
+        <v>userOffline</v>
       </c>
       <c r="B2" t="str">
-        <v>1</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="C2" t="str">
-        <v>laki-laki</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="D2" t="str">
-        <v>c</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="E2" t="str">
-        <v>a@a.com</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="F2" t="str">
-        <v>1</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="G2" t="str">
-        <v>2021-06-18T00:00:00Z</v>
+        <v>2021-08-27T00:00:00Z</v>
       </c>
       <c r="H2" t="str">
         <v>Kepaniteraan Hukum</v>
       </c>
       <c r="I2" t="str">
-        <v>09:00 - 10:00</v>
+        <v>14:00 - 15:00</v>
       </c>
       <c r="J2" t="str">
         <v>Waiting</v>
       </c>
-      <c r="K2">
-        <v>-525735</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
+      <c r="K2" t="str">
+        <v>0xc0002b4368</v>
+      </c>
+      <c r="L2" t="str">
+        <v>0xc0002b4380</v>
       </c>
       <c r="M2" t="str">
-        <v>0000-01-01 21:45:00 +0000 UTC</v>
+        <v>&lt;nil&gt;</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>a</v>
+        <v>userOffline</v>
       </c>
       <c r="B3" t="str">
-        <v>1</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="C3" t="str">
-        <v>laki-laki</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="D3" t="str">
-        <v>c</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="E3" t="str">
-        <v>a@a.com</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="F3" t="str">
-        <v>1</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="G3" t="str">
-        <v>2021-06-18T00:00:00Z</v>
+        <v>2021-08-27T00:00:00Z</v>
       </c>
       <c r="H3" t="str">
         <v>Kepaniteraan Pidana</v>
       </c>
       <c r="I3" t="str">
-        <v>09:00 - 10:00</v>
+        <v>14:00 - 15:00</v>
       </c>
       <c r="J3" t="str">
         <v>Waiting</v>
       </c>
-      <c r="K3">
-        <v>-525734</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
+      <c r="K3" t="str">
+        <v>0xc0002b43e0</v>
+      </c>
+      <c r="L3" t="str">
+        <v>0xc0002b43e8</v>
       </c>
       <c r="M3" t="str">
-        <v>0000-01-01 21:46:00 +0000 UTC</v>
+        <v>&lt;nil&gt;</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>a</v>
+        <v>userOffline</v>
       </c>
       <c r="B4" t="str">
-        <v>1</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="C4" t="str">
-        <v>laki-laki</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="D4" t="str">
-        <v>c</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="E4" t="str">
-        <v>a@a.com</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="F4" t="str">
-        <v>1</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="G4" t="str">
-        <v>2021-06-18T00:00:00Z</v>
+        <v>2021-08-27T00:00:00Z</v>
       </c>
       <c r="H4" t="str">
         <v>Upaya Hukum Perdata</v>
       </c>
       <c r="I4" t="str">
-        <v>09:00 - 10:00</v>
+        <v>14:00 - 15:00</v>
       </c>
       <c r="J4" t="str">
         <v>Waiting</v>
       </c>
-      <c r="K4">
-        <v>-525732</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
+      <c r="K4" t="str">
+        <v>0xc0002b4458</v>
+      </c>
+      <c r="L4" t="str">
+        <v>0xc0002b44a0</v>
       </c>
       <c r="M4" t="str">
-        <v>0000-01-01 21:48:00 +0000 UTC</v>
+        <v>&lt;nil&gt;</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>a</v>
+        <v>userOffline</v>
       </c>
       <c r="B5" t="str">
-        <v>1</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="C5" t="str">
-        <v>laki-laki</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="D5" t="str">
-        <v>c</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="E5" t="str">
-        <v>a@a.com</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="F5" t="str">
-        <v>1</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="G5" t="str">
-        <v>2021-06-18T00:00:00Z</v>
+        <v>2021-08-27T00:00:00Z</v>
       </c>
       <c r="H5" t="str">
-        <v>Salinan Putusan Perdata /Eksekusi</v>
+        <v>E-Court</v>
       </c>
       <c r="I5" t="str">
-        <v>09:00 - 10:00</v>
+        <v>14:00 - 15:00</v>
       </c>
       <c r="J5" t="str">
         <v>Waiting</v>
       </c>
-      <c r="K5">
-        <v>-525731</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
+      <c r="K5" t="str">
+        <v>0xc0002b4548</v>
+      </c>
+      <c r="L5" t="str">
+        <v>0xc0002b45a0</v>
       </c>
       <c r="M5" t="str">
-        <v>0000-01-01 21:49:00 +0000 UTC</v>
+        <v>&lt;nil&gt;</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>a</v>
+        <v>userOffline</v>
       </c>
       <c r="B6" t="str">
-        <v>1</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="C6" t="str">
-        <v>laki-laki</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="D6" t="str">
-        <v>c</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="E6" t="str">
-        <v>a@a.com</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="F6" t="str">
-        <v>1</v>
+        <v>&lt;nil&gt;</v>
       </c>
       <c r="G6" t="str">
-        <v>2021-06-18T00:00:00Z</v>
+        <v>2021-08-27T00:00:00Z</v>
       </c>
       <c r="H6" t="str">
-        <v>Umum &amp; Surat Masuk</v>
+        <v>E-Court</v>
       </c>
       <c r="I6" t="str">
-        <v>09:00 - 10:00</v>
+        <v>14:00 - 15:00</v>
       </c>
       <c r="J6" t="str">
         <v>Waiting</v>
       </c>
-      <c r="K6">
-        <v>-525730</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
+      <c r="K6" t="str">
+        <v>0xc0002b4648</v>
+      </c>
+      <c r="L6" t="str">
+        <v>0xc0002b4650</v>
       </c>
       <c r="M6" t="str">
-        <v>0000-01-01 21:50:00 +0000 UTC</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>a</v>
-      </c>
-      <c r="B7" t="str">
-        <v>1</v>
-      </c>
-      <c r="C7" t="str">
-        <v>laki-laki</v>
-      </c>
-      <c r="D7" t="str">
-        <v>c</v>
-      </c>
-      <c r="E7" t="str">
-        <v>a@a.com</v>
-      </c>
-      <c r="F7" t="str">
-        <v>1</v>
-      </c>
-      <c r="G7" t="str">
-        <v>2021-06-18T00:00:00Z</v>
-      </c>
-      <c r="H7" t="str">
-        <v>E-Court</v>
-      </c>
-      <c r="I7" t="str">
-        <v>09:00 - 10:00</v>
-      </c>
-      <c r="J7" t="str">
-        <v>Waiting</v>
-      </c>
-      <c r="K7">
-        <v>17</v>
-      </c>
-      <c r="L7">
-        <v>2</v>
-      </c>
-      <c r="M7" t="str">
-        <v>0000-01-01 13:17:00 +0000 UTC</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>a</v>
-      </c>
-      <c r="B8" t="str">
-        <v>1</v>
-      </c>
-      <c r="C8" t="str">
-        <v>laki-laki</v>
-      </c>
-      <c r="D8" t="str">
-        <v>c</v>
-      </c>
-      <c r="E8" t="str">
-        <v>a@a.com</v>
-      </c>
-      <c r="F8" t="str">
-        <v>1</v>
-      </c>
-      <c r="G8" t="str">
-        <v>2021-06-18T00:00:00Z</v>
-      </c>
-      <c r="H8" t="str">
-        <v>E-Court</v>
-      </c>
-      <c r="I8" t="str">
-        <v>09:00 - 10:00</v>
-      </c>
-      <c r="J8" t="str">
-        <v>Waiting</v>
-      </c>
-      <c r="K8">
-        <v>19</v>
-      </c>
-      <c r="L8">
-        <v>10</v>
-      </c>
-      <c r="M8" t="str">
-        <v>0000-01-01 13:19:00 +0000 UTC</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>a</v>
-      </c>
-      <c r="B9" t="str">
-        <v>1</v>
-      </c>
-      <c r="C9" t="str">
-        <v>laki-laki</v>
-      </c>
-      <c r="D9" t="str">
-        <v>c</v>
-      </c>
-      <c r="E9" t="str">
-        <v>a@a.com</v>
-      </c>
-      <c r="F9" t="str">
-        <v>1</v>
-      </c>
-      <c r="G9" t="str">
-        <v>2021-06-18T00:00:00Z</v>
-      </c>
-      <c r="H9" t="str">
-        <v>Pengaduan &amp; Infromasi</v>
-      </c>
-      <c r="I9" t="str">
-        <v>09:00 - 10:00</v>
-      </c>
-      <c r="J9" t="str">
-        <v>On Progress</v>
-      </c>
-      <c r="K9">
-        <v>43</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9" t="str">
-        <v>0000-01-01 09:43:00 +0000 UTC</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>a</v>
-      </c>
-      <c r="B10" t="str">
-        <v>1</v>
-      </c>
-      <c r="C10" t="str">
-        <v>laki-laki</v>
-      </c>
-      <c r="D10" t="str">
-        <v>c</v>
-      </c>
-      <c r="E10" t="str">
-        <v>a@a.com</v>
-      </c>
-      <c r="F10" t="str">
-        <v>1</v>
-      </c>
-      <c r="G10" t="str">
-        <v>2021-06-18T00:00:00Z</v>
-      </c>
-      <c r="H10" t="str">
-        <v>E-Court</v>
-      </c>
-      <c r="I10" t="str">
-        <v>09:00 - 10:00</v>
-      </c>
-      <c r="J10" t="str">
-        <v>On Progress</v>
-      </c>
-      <c r="K10">
-        <v>43</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="M10" t="str">
-        <v>0000-01-01 09:43:00 +0000 UTC</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>a</v>
-      </c>
-      <c r="B11" t="str">
-        <v>1</v>
-      </c>
-      <c r="C11" t="str">
-        <v>laki-laki</v>
-      </c>
-      <c r="D11" t="str">
-        <v>c</v>
-      </c>
-      <c r="E11" t="str">
-        <v>a@a.com</v>
-      </c>
-      <c r="F11" t="str">
-        <v>1</v>
-      </c>
-      <c r="G11" t="str">
-        <v>2021-06-18T00:00:00Z</v>
-      </c>
-      <c r="H11" t="str">
-        <v>E-Court</v>
-      </c>
-      <c r="I11" t="str">
-        <v>14:00 - 15:00</v>
-      </c>
-      <c r="J11" t="str">
-        <v>On Progress</v>
-      </c>
-      <c r="K11">
-        <v>5</v>
-      </c>
-      <c r="L11">
-        <v>2</v>
-      </c>
-      <c r="M11" t="str">
-        <v>0000-01-01 14:05:00 +0000 UTC</v>
+        <v>&lt;nil&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>